<commit_message>
add pay scale exception and other pay inputs to config files, modify contract_pay_year_and_raise function with default config file keyword arguments, adjust dependent scripts accordingly
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/pay_tables.xlsx
+++ b/seniority_list/excel/sample3/pay_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="1" state="visible" r:id="rId2"/>
@@ -243,8 +243,8 @@
   </sheetPr>
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>5</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>7</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>8</v>
@@ -3239,7 +3239,7 @@
   <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>3</v>
@@ -4218,7 +4218,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>4</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>5</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>6</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>7</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>8</v>
@@ -4438,7 +4438,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>9</v>
@@ -6479,7 +6479,7 @@
   <dimension ref="A1:N129"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -7986,7 +7986,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>2</v>
@@ -8030,7 +8030,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>3</v>
@@ -8074,7 +8074,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>4</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>5</v>
@@ -8162,7 +8162,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>6</v>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>7</v>
@@ -8250,7 +8250,7 @@
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>8</v>
@@ -8294,7 +8294,7 @@
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>9</v>
@@ -8338,7 +8338,7 @@
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>10</v>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="44" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>11</v>
@@ -8426,7 +8426,7 @@
     </row>
     <row r="45" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>12</v>
@@ -8470,7 +8470,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>13</v>
@@ -8514,7 +8514,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>14</v>
@@ -8558,7 +8558,7 @@
     </row>
     <row r="48" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>15</v>
@@ -8602,7 +8602,7 @@
     </row>
     <row r="49" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>16</v>
@@ -12182,8 +12182,8 @@
   </sheetPr>
   <dimension ref="A1:N137"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M54" activeCellId="0" sqref="M54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -13734,7 +13734,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -13778,7 +13778,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>2</v>
@@ -13822,7 +13822,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>3</v>
@@ -13866,7 +13866,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
@@ -13910,7 +13910,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>5</v>
@@ -13954,7 +13954,7 @@
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>6</v>
@@ -13998,7 +13998,7 @@
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>7</v>
@@ -14042,7 +14042,7 @@
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>8</v>
@@ -14086,7 +14086,7 @@
     </row>
     <row r="44" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>9</v>
@@ -14130,7 +14130,7 @@
     </row>
     <row r="45" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>10</v>
@@ -14174,7 +14174,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>11</v>
@@ -14218,7 +14218,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>12</v>
@@ -14262,7 +14262,7 @@
     </row>
     <row r="48" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>13</v>
@@ -14306,7 +14306,7 @@
     </row>
     <row r="49" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>14</v>
@@ -14350,7 +14350,7 @@
     </row>
     <row r="50" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>15</v>
@@ -14394,7 +14394,7 @@
     </row>
     <row r="51" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>16</v>
@@ -14438,7 +14438,7 @@
     </row>
     <row r="52" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>1950</v>
+        <v>2014.1</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>17</v>

</xml_diff>

<commit_message>
major upgrade to charting and dataset loading.  Add built-in filtering capability to most plotting functions.  Add load_datasets function
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/pay_tables.xlsx
+++ b/seniority_list/excel/sample3/pay_tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="basic_with_fur" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="enhanced_with_fur" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="basic" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="enhanced" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="basic_hours" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="enhanced_hours" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>

</xml_diff>

<commit_message>
major update of program for all spreadsheet input vs config files, removed case files folder and contents and config.py, added settings.xlsx, added 4 helper functions to functions module to assist with excel to python conversion, added make_color_list and add_pad plotting functions, modified all scripts and functions to work with new settings, color, and attribute dictionaries, added to and improved function docstrings
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/pay_tables.xlsx
+++ b/seniority_list/excel/sample3/pay_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rates" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -38,42 +38,46 @@
     <t xml:space="preserve">part_hours</t>
   </si>
   <si>
+    <t xml:space="preserve">full_pcnt</t>
+  </si>
+  <si>
     <t xml:space="preserve">jobstr</t>
   </si>
   <si>
-    <t xml:space="preserve">CA_4</t>
+    <t xml:space="preserve">Capt G4</t>
   </si>
   <si>
-    <t xml:space="preserve">CA_3</t>
+    <t xml:space="preserve">Capt G3</t>
   </si>
   <si>
-    <t xml:space="preserve">CA_2</t>
+    <t xml:space="preserve">Capt G2</t>
   </si>
   <si>
-    <t xml:space="preserve">FO_4</t>
+    <t xml:space="preserve">F/O G4</t>
   </si>
   <si>
-    <t xml:space="preserve">FO_3</t>
+    <t xml:space="preserve">F/O G3</t>
   </si>
   <si>
-    <t xml:space="preserve">FO_2</t>
+    <t xml:space="preserve">F/O G2</t>
   </si>
   <si>
-    <t xml:space="preserve">CA_1</t>
+    <t xml:space="preserve">Capt G1</t>
   </si>
   <si>
-    <t xml:space="preserve">FO_1</t>
+    <t xml:space="preserve">F/O G1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -156,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,6 +190,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3096,20 +3104,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65536"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3128,6 +3132,9 @@
       <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
@@ -3142,8 +3149,11 @@
       <c r="D2" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
+      <c r="E2" s="8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3159,8 +3169,11 @@
       <c r="D3" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>7</v>
+      <c r="E3" s="8" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3176,8 +3189,11 @@
       <c r="D4" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>8</v>
+      <c r="E4" s="8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3193,8 +3209,11 @@
       <c r="D5" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
+      <c r="E5" s="8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3210,8 +3229,11 @@
       <c r="D6" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>10</v>
+      <c r="E6" s="8" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3227,8 +3249,11 @@
       <c r="D7" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
+      <c r="E7" s="8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3244,8 +3269,11 @@
       <c r="D8" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
+      <c r="E8" s="8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3261,11 +3289,13 @@
       <c r="D9" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E9" s="8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>